<commit_message>
tried with IE. reverted back to Firefox.
</commit_message>
<xml_diff>
--- a/Selenium_NSE/test-data/TestData.xlsx
+++ b/Selenium_NSE/test-data/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="5040" windowWidth="11148" xWindow="2352" yWindow="1140"/>
+    <workbookView windowHeight="5040" windowWidth="11148" xWindow="2352" yWindow="1140" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Common" r:id="rId1" sheetId="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="2137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="2141">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -6467,70 +6467,82 @@
     <t>XPathsInPage</t>
   </si>
   <si>
+    <t>550.10</t>
+  </si>
+  <si>
+    <t>963.95</t>
+  </si>
+  <si>
+    <t>30.35</t>
+  </si>
+  <si>
+    <t>40.54</t>
+  </si>
+  <si>
+    <t>Mar 14, 09:58</t>
+  </si>
+  <si>
+    <t>857.50</t>
+  </si>
+  <si>
+    <t>4251</t>
+  </si>
+  <si>
+    <t>854.75</t>
+  </si>
+  <si>
+    <t>15058</t>
+  </si>
+  <si>
+    <t>851.50</t>
+  </si>
+  <si>
+    <t>875.00</t>
+  </si>
+  <si>
+    <t>3.36 K</t>
+  </si>
+  <si>
+    <t>11.40 K</t>
+  </si>
+  <si>
+    <t>11,754.03</t>
+  </si>
+  <si>
+    <t>24.94</t>
+  </si>
+  <si>
+    <t>10.17</t>
+  </si>
+  <si>
+    <t>2017 Mar 14, 09:59:31</t>
+  </si>
+  <si>
+    <t>2017-03-14 09:59:32.349</t>
+  </si>
+  <si>
     <t>Firefox</t>
   </si>
   <si>
-    <t>Mar 10, 15:59</t>
-  </si>
-  <si>
-    <t>861.30</t>
-  </si>
-  <si>
-    <t>11,011</t>
-  </si>
-  <si>
-    <t>861.25</t>
-  </si>
-  <si>
-    <t>116,405</t>
-  </si>
-  <si>
-    <t>843.40</t>
-  </si>
-  <si>
-    <t>863.85</t>
-  </si>
-  <si>
-    <t>550.10</t>
-  </si>
-  <si>
-    <t>963.95</t>
-  </si>
-  <si>
-    <t>1335</t>
-  </si>
-  <si>
-    <t>5497</t>
-  </si>
-  <si>
-    <t>11,850.34</t>
-  </si>
-  <si>
-    <t>30.35</t>
-  </si>
-  <si>
-    <t>28.38</t>
-  </si>
-  <si>
-    <t>40.54</t>
-  </si>
-  <si>
-    <t>25.15</t>
-  </si>
-  <si>
-    <t>10.25</t>
-  </si>
-  <si>
-    <t>2017 Mar 14, 00:07:02</t>
-  </si>
-  <si>
-    <t>2017-03-14 00:07:04.319</t>
-  </si>
-  <si>
-    <t>2017 Mar 14, 00:12:45</t>
-  </si>
-  <si>
-    <t>2017-03-14 00:12:47.271</t>
+    <t>Mar 14, 10:00</t>
+  </si>
+  <si>
+    <t>854.95</t>
+  </si>
+  <si>
+    <t>15231</t>
+  </si>
+  <si>
+    <t>3.79 K</t>
+  </si>
+  <si>
+    <t>11.06 K</t>
+  </si>
+  <si>
+    <t>2017 Mar 14, 10:01:04</t>
+  </si>
+  <si>
+    <t>2017-03-14 10:01:06.239</t>
   </si>
 </sst>
 </file>
@@ -7224,8 +7236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7277,13 +7289,13 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>2115</v>
+        <v>2133</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>2136</v>
+        <v>2140</v>
       </c>
     </row>
   </sheetData>
@@ -7294,6 +7306,11 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F2:F1048576" type="list">
+      <formula1>"IE, Chrome, Firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
@@ -7301,14 +7318,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK117"/>
+  <dimension ref="A1:AJ117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="AF80" xSplit="10" ySplit="1"/>
+    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="K80" xSplit="10" ySplit="1"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection activeCell="A2" pane="topRight" sqref="A2"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="AK82" pane="bottomRight" sqref="AK82"/>
+      <selection activeCell="A2" pane="bottomRight" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7321,7 +7338,7 @@
     <col min="6" max="6" customWidth="true" hidden="true" style="23" width="22.21875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" hidden="true" style="23" width="26.44140625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="23" width="11.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="23" width="9.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="23" width="13.44140625" collapsed="true"/>
     <col min="10" max="10" customWidth="true" style="23" width="9.33203125" collapsed="true"/>
     <col min="11" max="11" customWidth="true" style="23" width="14.33203125" collapsed="true"/>
     <col min="12" max="19" customWidth="true" style="23" width="12.44140625" collapsed="true"/>
@@ -7332,8 +7349,7 @@
     <col min="30" max="30" customWidth="true" style="23" width="5.44140625" collapsed="true"/>
     <col min="31" max="35" customWidth="true" style="23" width="16.109375" collapsed="true"/>
     <col min="36" max="36" customWidth="true" style="23" width="23.33203125" collapsed="true"/>
-    <col min="37" max="37" style="26" width="8.88671875" collapsed="false"/>
-    <col min="38" max="16384" style="26" width="8.88671875" collapsed="true"/>
+    <col min="37" max="16384" style="26" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" ht="55.2" r="1" s="28" spans="1:36" x14ac:dyDescent="0.3">
@@ -15724,58 +15740,58 @@
         <v>460</v>
       </c>
       <c r="I82" s="31" t="s">
+        <v>2134</v>
+      </c>
+      <c r="J82" t="s">
+        <v>2120</v>
+      </c>
+      <c r="K82" t="s">
+        <v>2121</v>
+      </c>
+      <c r="L82" t="s">
+        <v>2135</v>
+      </c>
+      <c r="M82" t="s">
+        <v>2136</v>
+      </c>
+      <c r="N82" t="s">
+        <v>2124</v>
+      </c>
+      <c r="O82" t="s">
+        <v>2125</v>
+      </c>
+      <c r="P82" t="s">
+        <v>2115</v>
+      </c>
+      <c r="Q82" t="s">
         <v>2116</v>
       </c>
-      <c r="J82" t="s">
+      <c r="R82" t="s">
+        <v>2137</v>
+      </c>
+      <c r="S82" t="s">
+        <v>2138</v>
+      </c>
+      <c r="T82" t="s">
+        <v>2128</v>
+      </c>
+      <c r="U82" t="s">
         <v>2117</v>
       </c>
-      <c r="K82" t="s">
+      <c r="V82" t="s">
+        <v>729</v>
+      </c>
+      <c r="W82" t="s">
         <v>2118</v>
       </c>
-      <c r="L82" t="s">
-        <v>2119</v>
-      </c>
-      <c r="M82" t="s">
-        <v>2120</v>
-      </c>
-      <c r="N82" t="s">
-        <v>2121</v>
-      </c>
-      <c r="O82" t="s">
-        <v>2122</v>
-      </c>
-      <c r="P82" t="s">
-        <v>2123</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>2124</v>
-      </c>
-      <c r="R82" t="s">
-        <v>2125</v>
-      </c>
-      <c r="S82" t="s">
-        <v>2126</v>
-      </c>
-      <c r="T82" t="s">
-        <v>2127</v>
-      </c>
-      <c r="U82" t="s">
-        <v>2128</v>
-      </c>
-      <c r="V82" t="s">
+      <c r="X82" t="s">
         <v>2129</v>
-      </c>
-      <c r="W82" t="s">
-        <v>2130</v>
-      </c>
-      <c r="X82" t="s">
-        <v>2131</v>
       </c>
       <c r="Y82" t="s">
         <v>469</v>
       </c>
       <c r="Z82" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
       <c r="AA82" t="s">
         <v>470</v>
@@ -15795,7 +15811,7 @@
       <c r="AH82" s="8"/>
       <c r="AI82" s="8"/>
       <c r="AJ82" t="s">
-        <v>2135</v>
+        <v>2139</v>
       </c>
     </row>
     <row customFormat="1" ht="55.2" r="83" s="29" spans="1:36" x14ac:dyDescent="0.3">
@@ -16066,7 +16082,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row customFormat="1" ht="55.2" r="86" s="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="69" r="86" s="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
         <v>5</v>
       </c>

</xml_diff>